<commit_message>
Updates and Name Update
</commit_message>
<xml_diff>
--- a/ConsumerGoods.xlsx
+++ b/ConsumerGoods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Finance\Anaylsen\Sectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F62F615-BB7C-48EC-8C95-4DD69C5C33A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0876E0-69D3-484B-B10B-33CAADAE179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="4290" windowWidth="38175" windowHeight="15240" activeTab="1" xr2:uid="{C5F9E374-3D8E-42B5-B067-E68CE63456D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21060" activeTab="1" xr2:uid="{C5F9E374-3D8E-42B5-B067-E68CE63456D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -51,6 +51,11 @@
     <externalReference r:id="rId34"/>
     <externalReference r:id="rId35"/>
     <externalReference r:id="rId36"/>
+    <externalReference r:id="rId37"/>
+    <externalReference r:id="rId38"/>
+    <externalReference r:id="rId39"/>
+    <externalReference r:id="rId40"/>
+    <externalReference r:id="rId41"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -132,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="1170">
   <si>
     <t>Consumer Goods</t>
   </si>
@@ -3636,6 +3641,12 @@
   </si>
   <si>
     <t>MOWI.OL</t>
+  </si>
+  <si>
+    <t>FQ425</t>
+  </si>
+  <si>
+    <t>Q225</t>
   </si>
 </sst>
 </file>
@@ -3885,6 +3896,45 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
+          <cell r="J2">
+            <v>52.07</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>28244.199404300001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>363.9</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>14201.6</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
           <cell r="I2">
             <v>81.52</v>
           </cell>
@@ -3911,7 +3961,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -3950,7 +4000,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -3989,7 +4039,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4028,7 +4078,163 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="J2">
+            <v>451.49</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>15459.684450730001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>304.32</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>4975.759</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="I2">
+            <v>164.28</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="I4">
+            <v>16076.2140936</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5">
+            <v>285.66300000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="I6">
+            <v>8.2520000000000007</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="J2">
+            <v>190.5</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>98509.662835499999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>200.3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>2094.9</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="J2">
+            <v>137.83000000000001</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>5880.7446451600008</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>312.92099999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>246.94499999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4067,7 +4273,46 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="H2">
+            <v>296.01</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="H4">
+            <v>211656.83751926999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="H5">
+            <v>1238</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="H6">
+            <v>38925</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4106,7 +4351,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4125,22 +4370,22 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="H2">
-            <v>74.5</v>
+            <v>92.6</v>
           </cell>
         </row>
         <row r="4">
           <cell r="H4">
-            <v>507.53855100000004</v>
+            <v>630.84657479999998</v>
           </cell>
         </row>
         <row r="5">
           <cell r="H5">
-            <v>110.736</v>
+            <v>110.125</v>
           </cell>
         </row>
         <row r="6">
           <cell r="H6">
-            <v>16.056000000000001</v>
+            <v>14.090999999999999</v>
           </cell>
         </row>
       </sheetData>
@@ -4155,7 +4400,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4194,7 +4439,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4233,7 +4478,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4272,46 +4517,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="H2">
-            <v>281</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="H4">
-            <v>201370.13176600001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5">
-            <v>1221</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6">
-            <v>39586</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4350,7 +4556,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4393,7 +4599,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4434,7 +4640,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4469,7 +4675,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4499,201 +4705,6 @@
         <row r="6">
           <cell r="H6">
             <v>26.78</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financials"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="J2">
-            <v>4080</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="J4">
-            <v>7244589.7719575036</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>1098839</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>1227407</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financials"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="I2">
-            <v>25.6</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="I4">
-            <v>22246.400000000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="I5">
-            <v>1078</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6">
-            <v>8797</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financials"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="I2">
-            <v>107400</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="I4">
-            <v>12361328.658</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="I5">
-            <v>1406213</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6">
-            <v>638981</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="I2">
-            <v>590</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="I4">
-            <v>68627665.371000007</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="I5">
-            <v>2695159</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6">
-            <v>76771</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="I3">
-            <v>69.63</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="I5">
-            <v>1232.2425974099999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6">
-            <v>33.557000000000002</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="I7">
-            <v>248.28200000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -4748,6 +4759,201 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Financials"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="J2">
+            <v>4080</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>7244589.7719575036</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>1098839</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>1227407</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financials"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="I2">
+            <v>25.6</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="I4">
+            <v>22246.400000000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5">
+            <v>1078</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="I6">
+            <v>8797</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financials"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="I2">
+            <v>107400</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="I4">
+            <v>12361328.658</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5">
+            <v>1406213</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="I6">
+            <v>638981</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="I2">
+            <v>590</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="I4">
+            <v>68627665.371000007</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5">
+            <v>2695159</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="I6">
+            <v>76771</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink34.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="I3">
+            <v>69.63</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5">
+            <v>1232.2425974099999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="I6">
+            <v>33.557000000000002</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="I7">
+            <v>248.28200000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink35.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
       <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
@@ -4779,7 +4985,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink36.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4793,22 +4999,22 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="J2">
-            <v>190.5</v>
+            <v>164.97</v>
           </cell>
         </row>
         <row r="4">
           <cell r="J4">
-            <v>98509.662835499999</v>
+            <v>33423.547236300001</v>
           </cell>
         </row>
         <row r="5">
           <cell r="J5">
-            <v>200.3</v>
+            <v>1515.252</v>
           </cell>
         </row>
         <row r="6">
           <cell r="J6">
-            <v>2094.9</v>
+            <v>5925.4940000000006</v>
           </cell>
         </row>
       </sheetData>
@@ -4832,22 +5038,22 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="H2">
-            <v>57.8</v>
+            <v>68.88</v>
           </cell>
         </row>
         <row r="4">
           <cell r="H4">
-            <v>77289.827881199992</v>
+            <v>89186.882892239984</v>
           </cell>
         </row>
         <row r="5">
           <cell r="H5">
-            <v>1517</v>
+            <v>1561</v>
           </cell>
         </row>
         <row r="6">
           <cell r="H6">
-            <v>19804</v>
+            <v>17624</v>
           </cell>
         </row>
       </sheetData>
@@ -6048,8 +6254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F34CF-7B93-4C80-9712-0C74998FDC34}">
   <dimension ref="A1:AG374"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6198,22 +6404,22 @@
       </c>
       <c r="E5" s="6">
         <f>+[2]Main!$H$2</f>
-        <v>281</v>
+        <v>296.01</v>
       </c>
       <c r="F5" s="4">
         <f>+[2]Main!$H$4</f>
-        <v>201370.13176600001</v>
+        <v>211656.83751926999</v>
       </c>
       <c r="G5" s="4">
         <f>+[2]Main!$H$6-[2]Main!$H$5</f>
-        <v>38365</v>
+        <v>37687</v>
       </c>
       <c r="H5" s="4">
         <f>+F5+G5</f>
-        <v>239735.13176600001</v>
+        <v>249343.83751926999</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>24</v>
+        <v>491</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -6278,22 +6484,22 @@
       </c>
       <c r="E7" s="6">
         <f>+[4]Main!$H$2</f>
-        <v>57.8</v>
+        <v>68.88</v>
       </c>
       <c r="F7" s="4">
         <f>+[4]Main!$H$4</f>
-        <v>77289.827881199992</v>
+        <v>89186.882892239984</v>
       </c>
       <c r="G7" s="4">
         <f>+[4]Main!$H$6-[4]Main!$H$5</f>
-        <v>18287</v>
+        <v>16063</v>
       </c>
       <c r="H7" s="4">
         <f>+F7+G7</f>
-        <v>95576.827881199992</v>
+        <v>105249.88289223998</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>24</v>
+        <v>491</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -6543,7 +6749,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C15" t="s">
@@ -6552,10 +6758,25 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="E15" s="6">
+        <f>+[10]Main!$J$2</f>
+        <v>52.07</v>
+      </c>
+      <c r="F15" s="4">
+        <f>+[10]Main!$J$4</f>
+        <v>28244.199404300001</v>
+      </c>
+      <c r="G15" s="4">
+        <f>+[10]Main!$J$6-[10]Main!$J$5</f>
+        <v>13837.7</v>
+      </c>
+      <c r="H15" s="4">
+        <f>+F15+G15</f>
+        <v>42081.899404299998</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>1168</v>
+      </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
@@ -6563,7 +6784,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C16" t="s">
@@ -6572,10 +6793,25 @@
       <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="E16" s="6">
+        <f>+[36]Main!$J$2</f>
+        <v>164.97</v>
+      </c>
+      <c r="F16" s="4">
+        <f>+[36]Main!$J$4</f>
+        <v>33423.547236300001</v>
+      </c>
+      <c r="G16" s="4">
+        <f>+[36]Main!$J$6-[36]Main!$J$5</f>
+        <v>4410.2420000000002</v>
+      </c>
+      <c r="H16" s="4">
+        <f>+F16+G16</f>
+        <v>37833.789236299999</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>491</v>
+      </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -6693,15 +6929,15 @@
         <v>27</v>
       </c>
       <c r="E22" s="6">
-        <f>+[10]Main!$I$2</f>
+        <f>+[11]Main!$I$2</f>
         <v>81.52</v>
       </c>
       <c r="F22" s="4">
-        <f>+[10]Main!$I$4</f>
+        <f>+[11]Main!$I$4</f>
         <v>28099.772318880001</v>
       </c>
       <c r="G22" s="4">
-        <f>+[10]Main!$I$6-[10]Main!$I$5</f>
+        <f>+[11]Main!$I$6-[11]Main!$I$5</f>
         <v>5160</v>
       </c>
       <c r="H22" s="4">
@@ -6798,15 +7034,15 @@
         <v>27</v>
       </c>
       <c r="E26" s="6">
-        <f>+[11]Main!$I$2</f>
+        <f>+[12]Main!$I$2</f>
         <v>51.28</v>
       </c>
       <c r="F26" s="4">
-        <f>+[11]Main!$I$4</f>
+        <f>+[12]Main!$I$4</f>
         <v>24539.198905600002</v>
       </c>
       <c r="G26" s="4">
-        <f>+[11]Main!$I$6-[11]Main!$I$5</f>
+        <f>+[12]Main!$I$6-[12]Main!$I$5</f>
         <v>1450</v>
       </c>
       <c r="H26" s="4">
@@ -6900,15 +7136,15 @@
         <v>27</v>
       </c>
       <c r="E30" s="6">
-        <f>+[12]Main!$J$2</f>
+        <f>+[13]Main!$J$2</f>
         <v>76.930000000000007</v>
       </c>
       <c r="F30" s="4">
-        <f>+[12]Main!$J$4</f>
+        <f>+[13]Main!$J$4</f>
         <v>20629.107760310002</v>
       </c>
       <c r="G30" s="4">
-        <f>+[12]Main!$J$6-[12]Main!$J$5</f>
+        <f>+[13]Main!$J$6-[13]Main!$J$5</f>
         <v>4155.7999999999993</v>
       </c>
       <c r="H30" s="4">
@@ -6939,15 +7175,15 @@
         <v>27</v>
       </c>
       <c r="E31" s="6">
-        <f>+[13]Main!$I$2</f>
+        <f>+[14]Main!$I$2</f>
         <v>192.3</v>
       </c>
       <c r="F31" s="4">
-        <f>+[13]Main!$I$4</f>
+        <f>+[14]Main!$I$4</f>
         <v>22527.326947800004</v>
       </c>
       <c r="G31" s="4">
-        <f>+[13]Main!$I$6-[13]Main!$I$5</f>
+        <f>+[14]Main!$I$6-[14]Main!$I$5</f>
         <v>2179.5999999999995</v>
       </c>
       <c r="H31" s="4">
@@ -7128,7 +7364,7 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C40" t="s">
@@ -7137,10 +7373,25 @@
       <c r="D40" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="E40" s="6">
+        <f>+[15]Main!$J$2</f>
+        <v>451.49</v>
+      </c>
+      <c r="F40" s="4">
+        <f>+[15]Main!$J$4</f>
+        <v>15459.684450730001</v>
+      </c>
+      <c r="G40" s="4">
+        <f>+[15]Main!$J$6-[15]Main!$J$5</f>
+        <v>4671.4390000000003</v>
+      </c>
+      <c r="H40" s="4">
+        <f>+F40+G40</f>
+        <v>20131.123450730003</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>491</v>
+      </c>
       <c r="Q40" s="4"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -7208,7 +7459,7 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C44" t="s">
@@ -7217,10 +7468,25 @@
       <c r="D44" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
+      <c r="E44" s="6">
+        <f>+[16]Main!$I$2</f>
+        <v>164.28</v>
+      </c>
+      <c r="F44" s="4">
+        <f>+[16]Main!$I$4</f>
+        <v>16076.2140936</v>
+      </c>
+      <c r="G44" s="4">
+        <f>+[16]Main!$I$6-[16]Main!$I$5</f>
+        <v>-277.411</v>
+      </c>
+      <c r="H44" s="4">
+        <f>+F44+G44</f>
+        <v>15798.8030936</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>491</v>
+      </c>
       <c r="Q44" s="4"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -7642,15 +7908,15 @@
         <v>172</v>
       </c>
       <c r="E66">
-        <f>+[31]Main!$J$2</f>
+        <f>+[17]Main!$J$2</f>
         <v>190.5</v>
       </c>
       <c r="F66" s="4">
-        <f>+[31]Main!$J$4*FX!C10</f>
+        <f>+[17]Main!$J$4*FX!C10</f>
         <v>9653.9469578789995</v>
       </c>
       <c r="G66" s="4">
-        <f>+([31]Main!$J$6-[31]Main!$J$5)*FX!C10</f>
+        <f>+([17]Main!$J$6-[17]Main!$J$5)*FX!C10</f>
         <v>185.67080000000001</v>
       </c>
       <c r="H66" s="4">
@@ -7762,7 +8028,7 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C72" t="s">
@@ -7771,9 +8037,25 @@
       <c r="D72" t="s">
         <v>27</v>
       </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
+      <c r="E72">
+        <f>+[18]Main!$J$2</f>
+        <v>137.83000000000001</v>
+      </c>
+      <c r="F72" s="4">
+        <f>+[18]Main!$J$4</f>
+        <v>5880.7446451600008</v>
+      </c>
+      <c r="G72" s="4">
+        <f>+[18]Main!$J$6-[18]Main!$J$5</f>
+        <v>-65.975999999999999</v>
+      </c>
+      <c r="H72" s="4">
+        <f>+F72+G72</f>
+        <v>5814.7686451600011</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>491</v>
+      </c>
       <c r="Q72" s="4"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -8836,15 +9118,15 @@
         <v>31</v>
       </c>
       <c r="E128">
-        <f>+[14]Main!$I$2</f>
+        <f>+[19]Main!$I$2</f>
         <v>15.7</v>
       </c>
       <c r="F128" s="4">
-        <f>+[14]Main!$I$4*FX!C3</f>
+        <f>+[19]Main!$I$4*FX!C3</f>
         <v>3243.4944</v>
       </c>
       <c r="G128" s="4">
-        <f>+([14]Main!$I$6-[14]Main!$I$5)*FX!C3</f>
+        <f>+([19]Main!$I$6-[19]Main!$I$5)*FX!C3</f>
         <v>2300.16</v>
       </c>
       <c r="H128" s="4">
@@ -10294,15 +10576,15 @@
         <v>172</v>
       </c>
       <c r="E203">
-        <f>+[15]Main!$J$2</f>
+        <f>+[20]Main!$J$2</f>
         <v>70.25</v>
       </c>
       <c r="F203" s="4">
-        <f>+[15]Main!$J$4*FX!C10</f>
+        <f>+[20]Main!$J$4*FX!C10</f>
         <v>772.74349442850007</v>
       </c>
       <c r="G203" s="4">
-        <f>+([15]Main!$J$6-[15]Main!$J$5)*FX!C10</f>
+        <f>+([20]Main!$J$6-[20]Main!$J$5)*FX!C10</f>
         <v>466.023124</v>
       </c>
       <c r="H203" s="4">
@@ -10367,26 +10649,26 @@
         <v>146</v>
       </c>
       <c r="E206">
-        <f>+[16]Main!$H$2</f>
-        <v>74.5</v>
+        <f>+[21]Main!$H$2</f>
+        <v>92.6</v>
       </c>
       <c r="F206" s="4">
-        <f>+[16]Main!$H$4*FX!C8</f>
-        <v>578.59394813999995</v>
+        <f>+[21]Main!$H$4*FX!C8</f>
+        <v>719.16509527199992</v>
       </c>
       <c r="G206" s="4">
-        <f>+([16]Main!$H$6-[16]Main!$H$5)*FX!C8</f>
-        <v>-107.93519999999999</v>
+        <f>+([21]Main!$H$6-[21]Main!$H$5)*FX!C8</f>
+        <v>-109.47875999999999</v>
       </c>
       <c r="H206" s="4">
         <f>+F206+G206</f>
-        <v>470.65874813999994</v>
+        <v>609.68633527199995</v>
       </c>
       <c r="I206" s="5" t="s">
-        <v>88</v>
+        <v>1169</v>
       </c>
       <c r="J206" s="9">
-        <v>45701</v>
+        <v>46066</v>
       </c>
       <c r="K206" s="5"/>
       <c r="L206" s="10">
@@ -11363,15 +11645,15 @@
         <v>926</v>
       </c>
       <c r="E259">
-        <f>+[17]Main!$J$2</f>
+        <f>+[22]Main!$J$2</f>
         <v>58.4</v>
       </c>
       <c r="F259" s="4">
-        <f>+[17]Main!$J$4*FX!C10</f>
+        <f>+[22]Main!$J$4*FX!C10</f>
         <v>501.81546996000003</v>
       </c>
       <c r="G259" s="4">
-        <f>+([17]Main!$J$6-[17]Main!$J$5)*FX!C10</f>
+        <f>+([22]Main!$J$6-[22]Main!$J$5)*FX!C10</f>
         <v>12.976179999999999</v>
       </c>
       <c r="H259" s="4">
@@ -12963,15 +13245,15 @@
         <v>926</v>
       </c>
       <c r="E348">
-        <f>+[18]Main!$I$2</f>
+        <f>+[23]Main!$I$2</f>
         <v>85</v>
       </c>
       <c r="F348" s="4">
-        <f>+[18]Main!$I$4*FX!C10</f>
+        <f>+[23]Main!$I$4*FX!C10</f>
         <v>302.45397000000003</v>
       </c>
       <c r="G348" s="4">
-        <f>+([18]Main!$I$6-[18]Main!$I$5)*FX!C10</f>
+        <f>+([23]Main!$I$6-[23]Main!$I$5)*FX!C10</f>
         <v>86.644348000000022</v>
       </c>
       <c r="H348" s="4">
@@ -13138,6 +13420,11 @@
     <hyperlink ref="B259" r:id="rId17" xr:uid="{1DE1AF70-501A-4EAF-BBBA-F2A52CC98387}"/>
     <hyperlink ref="B203" r:id="rId18" xr:uid="{333F9323-1D4E-4DED-99B8-123253F3C3FB}"/>
     <hyperlink ref="B66" r:id="rId19" xr:uid="{DD2F3985-F059-492A-ACBE-F18EDFF094EB}"/>
+    <hyperlink ref="B44" r:id="rId20" xr:uid="{B4DBE39C-E432-4F4E-8743-4B3B1FDF6A34}"/>
+    <hyperlink ref="B72" r:id="rId21" xr:uid="{4D631F33-B3DD-4E31-AFCB-3879505B9940}"/>
+    <hyperlink ref="B40" r:id="rId22" xr:uid="{943F80B6-F72B-4E85-AA19-F202B8F5955F}"/>
+    <hyperlink ref="B15" r:id="rId23" xr:uid="{018A53B6-FF7F-40C5-8DBC-8AF6CEADEA65}"/>
+    <hyperlink ref="B16" r:id="rId24" xr:uid="{4D5587CE-95E4-41FD-91DC-7D5D63A25FEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13148,7 +13435,7 @@
   <dimension ref="A1:P127"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13220,15 +13507,15 @@
         <v>27</v>
       </c>
       <c r="E4">
-        <f>+[19]Main!$I$2</f>
+        <f>+[24]Main!$I$2</f>
         <v>71.89</v>
       </c>
       <c r="F4" s="4">
-        <f>+[19]Main!$I$4</f>
+        <f>+[24]Main!$I$4</f>
         <v>309198.91839655</v>
       </c>
       <c r="G4" s="4">
-        <f>+[19]Main!$I$6-[19]Main!$I$5</f>
+        <f>+[24]Main!$I$6-[24]Main!$I$5</f>
         <v>28452</v>
       </c>
       <c r="H4" s="4">
@@ -13336,15 +13623,15 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <f>+[20]Main!$J$2</f>
+        <f>+[25]Main!$J$2</f>
         <v>97.02</v>
       </c>
       <c r="F9" s="4">
-        <f>+[20]Main!$J$4</f>
+        <f>+[25]Main!$J$4</f>
         <v>110205.01800000001</v>
       </c>
       <c r="G9" s="4">
-        <f>+[20]Main!$J$6-[20]Main!$J$5</f>
+        <f>+[25]Main!$J$6-[25]Main!$J$5</f>
         <v>11604.2</v>
       </c>
       <c r="H9" s="4">
@@ -15631,15 +15918,15 @@
         <v>27</v>
       </c>
       <c r="E5" s="16">
-        <f>+[21]Main!$K$3</f>
+        <f>+[26]Main!$K$3</f>
         <v>168.82</v>
       </c>
       <c r="F5" s="4">
-        <f>+[21]Main!$K$5</f>
+        <f>+[26]Main!$K$5</f>
         <v>262490.99604921998</v>
       </c>
       <c r="G5" s="4">
-        <f>+[21]Main!$K$7-[21]Main!$K$6</f>
+        <f>+[26]Main!$K$7-[26]Main!$K$6</f>
         <v>41479</v>
       </c>
       <c r="H5" s="4">
@@ -15692,15 +15979,15 @@
         <v>27</v>
       </c>
       <c r="E6" s="16">
-        <f>+[22]Main!$M$3</f>
+        <f>+[27]Main!$M$3</f>
         <v>58.4</v>
       </c>
       <c r="F6" s="4">
-        <f>+[22]Main!$M$5</f>
+        <f>+[27]Main!$M$5</f>
         <v>98371.986171199998</v>
       </c>
       <c r="G6" s="4">
-        <f>+[22]Main!$M$7-[22]Main!$M$6</f>
+        <f>+[27]Main!$M$7-[27]Main!$M$6</f>
         <v>21333</v>
       </c>
       <c r="H6" s="4">
@@ -15753,15 +16040,15 @@
         <v>31</v>
       </c>
       <c r="E7" s="16">
-        <f>+[23]Main!$H$2</f>
+        <f>+[28]Main!$H$2</f>
         <v>38.49</v>
       </c>
       <c r="F7" s="4">
-        <f>+[23]Main!$H$5*FX!C3</f>
+        <f>+[28]Main!$H$5*FX!C3</f>
         <v>93986.9568</v>
       </c>
       <c r="G7" s="4">
-        <f>+([22]Main!$M$7-[22]Main!$M$6)*FX!C3</f>
+        <f>+([27]Main!$M$7-[27]Main!$M$6)*FX!C3</f>
         <v>27306.240000000002</v>
       </c>
       <c r="H7" s="4">
@@ -15809,15 +16096,15 @@
         <v>40</v>
       </c>
       <c r="E8" s="16">
-        <f>+[24]Main!$H$2</f>
+        <f>+[29]Main!$H$2</f>
         <v>485.4</v>
       </c>
       <c r="F8" s="4">
-        <f>+[24]Main!$H$4*FX!C4</f>
+        <f>+[29]Main!$H$4*FX!C4</f>
         <v>72888.393927045603</v>
       </c>
       <c r="G8" s="4">
-        <f>+([24]Main!$H$6-[24]Main!$H$5)*FX!C4</f>
+        <f>+([29]Main!$H$6-[29]Main!$H$5)*FX!C4</f>
         <v>-228.87708000000006</v>
       </c>
       <c r="H8" s="4">
@@ -15854,15 +16141,15 @@
         <v>95</v>
       </c>
       <c r="E9" s="4">
-        <f>+[25]Main!$J$2</f>
+        <f>+[30]Main!$J$2</f>
         <v>4080</v>
       </c>
       <c r="F9" s="4">
-        <f>+[25]Main!$J$4*FX!C5</f>
+        <f>+[30]Main!$J$4*FX!C5</f>
         <v>49263.210449311024</v>
       </c>
       <c r="G9" s="4">
-        <f>+([25]Main!$J$6-[25]Main!$J$5)*FX!C5</f>
+        <f>+([30]Main!$J$6-[30]Main!$J$5)*FX!C5</f>
         <v>874.26239999999996</v>
       </c>
       <c r="H9" s="4">
@@ -15904,15 +16191,15 @@
         <v>31</v>
       </c>
       <c r="E10" s="16">
-        <f>+[26]Main!$I$2</f>
+        <f>+[31]Main!$I$2</f>
         <v>25.6</v>
       </c>
       <c r="F10" s="4">
-        <f>+([26]Main!$I$4)*FX!C3</f>
+        <f>+([31]Main!$I$4)*FX!C3</f>
         <v>28475.392000000003</v>
       </c>
       <c r="G10" s="4">
-        <f>+([26]Main!$I$6-[26]Main!$I$5)*FX!C3</f>
+        <f>+([31]Main!$I$6-[31]Main!$I$5)*FX!C3</f>
         <v>9880.32</v>
       </c>
       <c r="H10" s="4">
@@ -15948,15 +16235,15 @@
         <v>617</v>
       </c>
       <c r="E11" s="4">
-        <f>+[27]Main!$I$2</f>
+        <f>+[32]Main!$I$2</f>
         <v>107400</v>
       </c>
       <c r="F11" s="4">
-        <f>+[27]Main!$I$4*FX!C6</f>
+        <f>+[32]Main!$I$4*FX!C6</f>
         <v>9270.9964935000007</v>
       </c>
       <c r="G11" s="4">
-        <f>+([27]Main!$I$6-[27]Main!$I$5)*FX!C6</f>
+        <f>+([32]Main!$I$6-[32]Main!$I$5)*FX!C6</f>
         <v>-575.42399999999998</v>
       </c>
       <c r="H11" s="4">
@@ -15990,15 +16277,15 @@
         <v>240</v>
       </c>
       <c r="E12" s="4">
-        <f>+[28]Main!$I$2</f>
+        <f>+[33]Main!$I$2</f>
         <v>590</v>
       </c>
       <c r="F12" s="4">
-        <f>+[28]Main!$I$4*FX!C7</f>
+        <f>+[33]Main!$I$4*FX!C7</f>
         <v>4254.915253002001</v>
       </c>
       <c r="G12" s="4">
-        <f>+([28]Main!$I$6-[28]Main!$I$5)*FX!C7</f>
+        <f>+([33]Main!$I$6-[33]Main!$I$5)*FX!C7</f>
         <v>-162.340056</v>
       </c>
       <c r="H12" s="4">
@@ -16177,15 +16464,15 @@
         <v>27</v>
       </c>
       <c r="E19" s="16">
-        <f>+[29]Main!$I$3</f>
+        <f>+[34]Main!$I$3</f>
         <v>69.63</v>
       </c>
       <c r="F19" s="4">
-        <f>+[29]Main!$I$5</f>
+        <f>+[34]Main!$I$5</f>
         <v>1232.2425974099999</v>
       </c>
       <c r="G19" s="4">
-        <f>+[29]Main!$I$7-[29]Main!$I$6</f>
+        <f>+[34]Main!$I$7-[34]Main!$I$6</f>
         <v>214.72500000000002</v>
       </c>
       <c r="H19" s="4">
@@ -16219,15 +16506,15 @@
         <v>27</v>
       </c>
       <c r="E20" s="16">
-        <f>+[30]Main!$I$2</f>
+        <f>+[35]Main!$I$2</f>
         <v>4.3600000000000003</v>
       </c>
       <c r="F20" s="4">
-        <f>+[30]Main!$I$4</f>
+        <f>+[35]Main!$I$4</f>
         <v>248.91663792000003</v>
       </c>
       <c r="G20" s="4">
-        <f>+[30]Main!$I$6-[30]Main!$I$5</f>
+        <f>+[35]Main!$I$6-[35]Main!$I$5</f>
         <v>-34.395385999999995</v>
       </c>
       <c r="H20" s="4">

</xml_diff>